<commit_message>
added countColor function, changed relation between GameUI and GameLogic to composition instead by reference
</commit_message>
<xml_diff>
--- a/pytest_files/board.xlsx
+++ b/pytest_files/board.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymond\Documents\code\python\Othello_AI\pytest_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B7F4DE-B42E-4113-9992-05638105BD37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF21383-67FB-4F02-96B7-46CECB2F327D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="4875" windowWidth="5910" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11017" yWindow="3983" windowWidth="5910" windowHeight="9524" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="3">
   <si>
     <t>B</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>UB</t>
   </si>
 </sst>
 </file>
@@ -388,7 +385,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -457,7 +454,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>

</xml_diff>